<commit_message>
formatted an OA list
</commit_message>
<xml_diff>
--- a/outputs/complete_lists/Older Adults/OA S016.xlsx
+++ b/outputs/complete_lists/Older Adults/OA S016.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amuller\Desktop\Alana\UA\R_projects\inflatable-project\outputs\complete_lists\Older Adults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4906AE08-43A7-4D84-AA00-394BE7E34EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3247C9-47B4-4A50-97B1-17C0EEA746D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42200" yWindow="3350" windowWidth="21260" windowHeight="18260"/>
+    <workbookView xWindow="10830" yWindow="1370" windowWidth="26200" windowHeight="18260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ten_lists" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="141">
   <si>
     <t>DD_#</t>
   </si>
@@ -424,9 +424,6 @@
     <t>trophy</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>walk/same</t>
   </si>
   <si>
@@ -437,12 +434,21 @@
   </si>
   <si>
     <t>no walk/diff</t>
+  </si>
+  <si>
+    <t>S016 OA</t>
+  </si>
+  <si>
+    <t>start DD</t>
+  </si>
+  <si>
+    <t>start SD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -760,7 +766,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -875,6 +881,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -920,8 +941,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1276,796 +1298,781 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="1.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" t="s">
+        <v>139</v>
+      </c>
+      <c r="I3" t="s">
+        <v>137</v>
+      </c>
+      <c r="K3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="H5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="H6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="H7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E8" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="H8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" t="s">
+        <v>140</v>
+      </c>
+      <c r="I10" t="s">
+        <v>134</v>
+      </c>
+      <c r="K10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E11" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="G11">
+        <v>7</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E12" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="H12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E13" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="H13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E14" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="H14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E15" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="H15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>134</v>
+      </c>
+      <c r="E17" t="s">
+        <v>139</v>
+      </c>
+      <c r="I17" t="s">
+        <v>137</v>
+      </c>
+      <c r="K17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E18" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="G18">
+        <v>8</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E19" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="H19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E20" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="H20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E21" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="H21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B22" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E22" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="H22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>137</v>
+      </c>
+      <c r="E24" t="s">
+        <v>140</v>
+      </c>
+      <c r="I24" t="s">
+        <v>134</v>
+      </c>
+      <c r="K24" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C25" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E25" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="G25">
+        <v>9</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D26" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E26" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="H26" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B27" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C27" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D27" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E27" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="H27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B28" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C28" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D28" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E28" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="H28" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B29" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C29" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D29" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E29" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="H29" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C31" t="s">
+        <v>135</v>
+      </c>
+      <c r="E31" t="s">
+        <v>140</v>
+      </c>
+      <c r="I31" t="s">
+        <v>136</v>
+      </c>
+      <c r="K31" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C32" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D32" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E32" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="G32">
+        <v>10</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B33" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C33" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D33" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E33" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="H33" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B34" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C34" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D34" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E34" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="H34" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B35" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C35" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D35" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E35" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="H35" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B36" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C36" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D36" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E36" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>77</v>
-      </c>
-      <c r="B32" t="s">
-        <v>78</v>
-      </c>
-      <c r="C32" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>80</v>
-      </c>
-      <c r="B33" t="s">
-        <v>81</v>
-      </c>
-      <c r="C33" t="s">
-        <v>82</v>
-      </c>
-      <c r="D33" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>43</v>
-      </c>
-      <c r="B34" t="s">
-        <v>84</v>
-      </c>
-      <c r="C34" t="s">
-        <v>43</v>
-      </c>
-      <c r="D34" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>86</v>
-      </c>
-      <c r="B35" t="s">
-        <v>87</v>
-      </c>
-      <c r="C35" t="s">
-        <v>46</v>
-      </c>
-      <c r="D35" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" t="s">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" t="s">
-        <v>89</v>
-      </c>
-      <c r="C38" t="s">
-        <v>65</v>
-      </c>
-      <c r="D38" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>91</v>
-      </c>
-      <c r="B39" t="s">
-        <v>92</v>
-      </c>
-      <c r="C39" t="s">
-        <v>68</v>
-      </c>
-      <c r="D39" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>29</v>
-      </c>
-      <c r="B40" t="s">
-        <v>94</v>
-      </c>
-      <c r="C40" t="s">
-        <v>13</v>
-      </c>
-      <c r="D40" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>96</v>
-      </c>
-      <c r="B41" t="s">
-        <v>97</v>
-      </c>
-      <c r="C41" t="s">
-        <v>31</v>
-      </c>
-      <c r="D41" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>0</v>
-      </c>
-      <c r="B43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C43" t="s">
-        <v>2</v>
-      </c>
-      <c r="D43" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>99</v>
-      </c>
-      <c r="B44" t="s">
-        <v>100</v>
-      </c>
-      <c r="C44" t="s">
-        <v>101</v>
-      </c>
-      <c r="D44" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>103</v>
-      </c>
-      <c r="B45" t="s">
-        <v>104</v>
-      </c>
-      <c r="C45" t="s">
-        <v>105</v>
-      </c>
-      <c r="D45" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>41</v>
-      </c>
-      <c r="B46" t="s">
-        <v>107</v>
-      </c>
-      <c r="C46" t="s">
-        <v>108</v>
-      </c>
-      <c r="D46" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>96</v>
-      </c>
-      <c r="B47" t="s">
-        <v>110</v>
-      </c>
-      <c r="C47" t="s">
-        <v>86</v>
-      </c>
-      <c r="D47" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>0</v>
-      </c>
-      <c r="B49" t="s">
-        <v>1</v>
-      </c>
-      <c r="C49" t="s">
-        <v>2</v>
-      </c>
-      <c r="D49" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>112</v>
-      </c>
-      <c r="B50" t="s">
-        <v>113</v>
-      </c>
-      <c r="C50" t="s">
-        <v>36</v>
-      </c>
-      <c r="D50" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>68</v>
-      </c>
-      <c r="B51" t="s">
-        <v>115</v>
-      </c>
-      <c r="C51" t="s">
-        <v>91</v>
-      </c>
-      <c r="D51" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>117</v>
-      </c>
-      <c r="B52" t="s">
-        <v>118</v>
-      </c>
-      <c r="C52" t="s">
-        <v>43</v>
-      </c>
-      <c r="D52" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>120</v>
-      </c>
-      <c r="B53" t="s">
-        <v>121</v>
-      </c>
-      <c r="C53" t="s">
-        <v>75</v>
-      </c>
-      <c r="D53" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>0</v>
-      </c>
-      <c r="B55" t="s">
-        <v>1</v>
-      </c>
-      <c r="C55" t="s">
-        <v>2</v>
-      </c>
-      <c r="D55" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>123</v>
-      </c>
-      <c r="B56" t="s">
-        <v>124</v>
-      </c>
-      <c r="C56" t="s">
-        <v>19</v>
-      </c>
-      <c r="D56" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>103</v>
-      </c>
-      <c r="B57" t="s">
-        <v>126</v>
-      </c>
-      <c r="C57" t="s">
-        <v>103</v>
-      </c>
-      <c r="D57" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>128</v>
-      </c>
-      <c r="B58" t="s">
-        <v>129</v>
-      </c>
-      <c r="C58" t="s">
-        <v>41</v>
-      </c>
-      <c r="D58" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
+      <c r="H36" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B59" t="s">
+      <c r="I36" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C59" t="s">
+      <c r="J36" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D59" t="s">
+      <c r="K36" s="1" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B61" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62">
-        <v>1</v>
-      </c>
-      <c r="B62" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63">
-        <v>2</v>
-      </c>
-      <c r="B63" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A64">
-        <v>3</v>
-      </c>
-      <c r="B64" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65">
-        <v>4</v>
-      </c>
-      <c r="B65" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A66">
-        <v>5</v>
-      </c>
-      <c r="B66" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A67">
-        <v>6</v>
-      </c>
-      <c r="B67" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A68">
-        <v>7</v>
-      </c>
-      <c r="B68" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A69">
-        <v>8</v>
-      </c>
-      <c r="B69" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A70">
-        <v>9</v>
-      </c>
-      <c r="B70" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A71">
-        <v>10</v>
-      </c>
-      <c r="B71" t="s">
-        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new lists for OA inflatables
</commit_message>
<xml_diff>
--- a/outputs/complete_lists/Older Adults/OA S016.xlsx
+++ b/outputs/complete_lists/Older Adults/OA S016.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amuller\Desktop\Alana\UA\R_projects\inflatable-project\outputs\complete_lists\Older Adults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3247C9-47B4-4A50-97B1-17C0EEA746D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC1DC06-484A-4A41-8D62-D6D1FE6BCB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10830" yWindow="1370" windowWidth="26200" windowHeight="18260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16260" yWindow="2480" windowWidth="21620" windowHeight="18090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ten_lists" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="139">
   <si>
     <t>DD_#</t>
   </si>
@@ -130,9 +130,6 @@
     <t>starfish</t>
   </si>
   <si>
-    <t>A3</t>
-  </si>
-  <si>
     <t>globe</t>
   </si>
   <si>
@@ -190,9 +187,6 @@
     <t>lobster</t>
   </si>
   <si>
-    <t>A7</t>
-  </si>
-  <si>
     <t>baby bottle</t>
   </si>
   <si>
@@ -253,9 +247,6 @@
     <t>parrot</t>
   </si>
   <si>
-    <t>A1</t>
-  </si>
-  <si>
     <t>bread</t>
   </si>
   <si>
@@ -373,9 +364,6 @@
     <t>gummy bear</t>
   </si>
   <si>
-    <t>A8</t>
-  </si>
-  <si>
     <t>flower</t>
   </si>
   <si>
@@ -443,6 +431,12 @@
   </si>
   <si>
     <t>start SD</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>B8</t>
   </si>
 </sst>
 </file>
@@ -1302,7 +1296,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1322,21 +1316,21 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="F1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="I3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -1385,16 +1379,16 @@
         <v>7</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -1411,16 +1405,16 @@
         <v>10</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -1437,16 +1431,16 @@
         <v>14</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -1463,30 +1457,30 @@
         <v>18</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
+        <v>131</v>
+      </c>
+      <c r="E10" t="s">
+        <v>136</v>
+      </c>
+      <c r="I10" t="s">
+        <v>130</v>
+      </c>
+      <c r="K10" t="s">
         <v>135</v>
-      </c>
-      <c r="E10" t="s">
-        <v>140</v>
-      </c>
-      <c r="I10" t="s">
-        <v>134</v>
-      </c>
-      <c r="K10" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -1535,16 +1529,16 @@
         <v>22</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -1561,16 +1555,16 @@
         <v>26</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -1590,13 +1584,13 @@
         <v>29</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -1613,30 +1607,30 @@
         <v>34</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E17" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="I17" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K17" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -1679,74 +1673,74 @@
         <v>35</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="H19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K20" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="H21" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
@@ -1754,39 +1748,39 @@
         <v>33</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="H22" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E24" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="I24" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="K24" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
@@ -1823,120 +1817,120 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="H26" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="H27" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B28" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="H28" s="1" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="H29" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C31" t="s">
+        <v>131</v>
+      </c>
+      <c r="E31" t="s">
+        <v>136</v>
+      </c>
+      <c r="I31" t="s">
+        <v>132</v>
+      </c>
+      <c r="K31" t="s">
         <v>135</v>
-      </c>
-      <c r="E31" t="s">
-        <v>140</v>
-      </c>
-      <c r="I31" t="s">
-        <v>136</v>
-      </c>
-      <c r="K31" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
@@ -1973,106 +1967,106 @@
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B33" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="H33" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B34" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="H34" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B35" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="H35" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B36" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="H36" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>